<commit_message>
Added test for adjacency list of a room cell that is not the center
</commit_message>
<xml_diff>
--- a/data/ClueLayoutTests.xlsx
+++ b/data/ClueLayoutTests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rj\Fall_2022_Courses\Software_Engineering\ClueGame\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE5D75F-9573-4D7C-99F0-CD30999F9A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0ECB95-E42F-499B-95B0-226CCA67EA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -172,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,6 +263,12 @@
         <bgColor rgb="FFFCE5CD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -276,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -340,6 +346,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,7 +576,7 @@
   <dimension ref="A1:AB1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1538,7 @@
       <c r="F12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="22" t="s">
         <v>26</v>
       </c>
       <c r="H12" s="4" t="s">

</xml_diff>